<commit_message>
Update reannotation script and documentation
</commit_message>
<xml_diff>
--- a/scripts/processing/output/reannotation.xlsx
+++ b/scripts/processing/output/reannotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/scripts/processing/output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xpragm/code/github/mol-mod/scripts/processing/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E67EE44-B476-C542-A1E8-50AAD2243C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3D24BC-1972-364F-810E-B385B02FE317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="3940" windowWidth="25580" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6400" yWindow="5820" windowWidth="33040" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="74">
   <si>
     <t>asv_sequence</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>sp015660815</t>
+  </si>
+  <si>
+    <t>XXX</t>
   </si>
 </sst>
 </file>
@@ -584,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -666,7 +669,7 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>

</xml_diff>